<commit_message>
fix: adding new subawardBulkUpload.xlsx and generated outputTemplates.json
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/subawardBulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/subawardBulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\Downloads\SLFRFBulkUploadTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\do.treas.gov\dfsres\isilon\Homeshare3\CarrikerCh\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93700437-54C7-442F-B804-12B87FE85BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDE387B-F620-43D9-9B60-E28F315974D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="855" windowWidth="20655" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Award-Reporting-Master" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>Template Name: Subaward Reporting</t>
   </si>
@@ -280,30 +280,38 @@
  "Other"</t>
   </si>
   <si>
-    <t>The Subrecipient's or Contractor's Unique Entity Identifier (UEI) from their SAM.gov profile. 
+    <t>Conditional</t>
+  </si>
+  <si>
+    <t>Explaination if Primary Sector response is "Other"
+Max characters 100</t>
+  </si>
+  <si>
+    <t>Version: 2023.02.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Subrecipient's, Contractor's, or Beneficiary's  Internal Revenue Service (IRS) Taxpayer Identification Number. 
+Format XXXXXXXXX, 
+9 numeric characters.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Subrecipient's or Contractor's Unique Entity Identifier (UEI) from their SAM.gov profile. 
 Format XXXXXXXXXXXX, 
 12 alpha-numeric characters.
-NOTE: One of the following identification numbers must be provided:
--UEI, or
--TIN</t>
-  </si>
-  <si>
-    <t>The Subrecipient's, Contractor's, or Beneficiary's  Internal Revenue Service (IRS) Taxpayer Identification Number. 
-Format XXXXXXXXX, 
-9 numeric characters.
-NOTE: One of the following identification numbers must be provided:
--UEI, or
--TIN</t>
-  </si>
-  <si>
-    <t>Conditional</t>
-  </si>
-  <si>
-    <t>Explaination if Primary Sector response is "Other"
-Max characters 100</t>
-  </si>
-  <si>
-    <t>Version: 2022.12.13</t>
+</t>
+  </si>
+  <si>
+    <t>SubAward/Direct Payment Entity Type</t>
+  </si>
+  <si>
+    <t>The type of entity for this subaward or direct payment. Select one of the predefined menu items:
+"Subrecipient"
+"Contractor"
+"Beneficiary"</t>
+  </si>
+  <si>
+    <t>Entity_Type_2__c</t>
   </si>
 </sst>
 </file>
@@ -348,7 +356,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -412,24 +420,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -458,11 +453,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -680,39 +676,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U979"/>
+  <dimension ref="A1:V979"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.125" customWidth="1"/>
     <col min="2" max="3" width="18.625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.875" customWidth="1"/>
-    <col min="5" max="5" width="186" customWidth="1"/>
-    <col min="6" max="6" width="32.875" customWidth="1"/>
-    <col min="7" max="7" width="25.625" customWidth="1"/>
-    <col min="8" max="8" width="24.25" style="2" customWidth="1"/>
-    <col min="9" max="9" width="76" customWidth="1"/>
-    <col min="10" max="10" width="30.125" customWidth="1"/>
-    <col min="11" max="11" width="67.875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="24.125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="72.625" customWidth="1"/>
-    <col min="14" max="14" width="74.875" customWidth="1"/>
-    <col min="15" max="15" width="28.5" customWidth="1"/>
-    <col min="16" max="16" width="23.625" customWidth="1"/>
-    <col min="17" max="17" width="27.5" customWidth="1"/>
-    <col min="18" max="18" width="22.875" customWidth="1"/>
-    <col min="19" max="19" width="24.625" customWidth="1"/>
-    <col min="20" max="20" width="27.5" customWidth="1"/>
-    <col min="21" max="21" width="44.75" customWidth="1"/>
+    <col min="4" max="4" width="44.5" customWidth="1"/>
+    <col min="5" max="6" width="39.75" customWidth="1"/>
+    <col min="7" max="7" width="32.875" customWidth="1"/>
+    <col min="8" max="8" width="25.625" customWidth="1"/>
+    <col min="9" max="9" width="24.25" style="2" customWidth="1"/>
+    <col min="10" max="10" width="76" customWidth="1"/>
+    <col min="11" max="11" width="30.125" customWidth="1"/>
+    <col min="12" max="12" width="67.875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="24.125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="72.625" customWidth="1"/>
+    <col min="15" max="15" width="74.875" customWidth="1"/>
+    <col min="16" max="16" width="28.5" customWidth="1"/>
+    <col min="17" max="17" width="23.625" customWidth="1"/>
+    <col min="18" max="18" width="27.5" customWidth="1"/>
+    <col min="19" max="19" width="22.875" customWidth="1"/>
+    <col min="20" max="20" width="24.625" customWidth="1"/>
+    <col min="21" max="21" width="27.5" customWidth="1"/>
+    <col min="22" max="22" width="44.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -720,12 +716,12 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="7"/>
+      <c r="K1" s="6"/>
       <c r="L1" s="7"/>
-      <c r="M1" s="6"/>
+      <c r="M1" s="7"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -733,8 +729,9 @@
       <c r="R1" s="6"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -744,12 +741,12 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
+      <c r="K2" s="6"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="6"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
@@ -757,8 +754,9 @@
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>62</v>
       </c>
@@ -768,12 +766,12 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="7"/>
+      <c r="K3" s="6"/>
       <c r="L3" s="7"/>
-      <c r="M3" s="6"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
@@ -781,8 +779,9 @@
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -798,61 +797,64 @@
       <c r="E4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="R4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="S4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="T4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="U4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="V4" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>38</v>
@@ -863,38 +865,38 @@
       <c r="E5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="18" t="s">
         <v>37</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>67</v>
+      <c r="I5" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>37</v>
+        <v>65</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="M5" s="11" t="s">
         <v>37</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>38</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="9" t="s">
         <v>37</v>
@@ -903,20 +905,23 @@
         <v>37</v>
       </c>
       <c r="S5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="T5" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="U5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="V5" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="31.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="31.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -928,64 +933,67 @@
       <c r="E6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="M6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="N6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="R6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="U6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="V6" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="1" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" s="1" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>66</v>
+      <c r="B7" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>40</v>
@@ -993,56 +1001,59 @@
       <c r="E7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="J7" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="K7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="N7" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="O7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="P7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="Q7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="R7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="S7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="S7" s="12" t="s">
+      <c r="T7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="T7" s="12" t="s">
+      <c r="U7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="U7" s="12" t="s">
+      <c r="V7" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1050,12 +1061,12 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="6"/>
+      <c r="M8" s="7"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
@@ -1063,21 +1074,22 @@
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="6"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -1085,14 +1097,15 @@
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
1028 subaward entity type (#1109)
feat: new subaward/direct payments entity type (#1028)

Adds entityType for Subaward

* fix: Runs npx eslint --fix on generateRules. This is the automated portion.
* fix: Manually-applied remaining eslint fixes
* fix: Adding script alias and VSCode Debug target to run it for generateRules
* fix: update launch.json to use yarn commands
* fix: updating environment.js
* fix: adding generated templateRules.json
* fix: adding new subawardBulkUpload.xlsx and generated outputTemplates.json
* fix: force-adding xlsm file
---------

Co-authored-by: aditya <asridhar@usdigitalresponse.org>
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/subawardBulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/subawardBulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\Downloads\SLFRFBulkUploadTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\do.treas.gov\dfsres\isilon\Homeshare3\CarrikerCh\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93700437-54C7-442F-B804-12B87FE85BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDE387B-F620-43D9-9B60-E28F315974D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="855" windowWidth="20655" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Award-Reporting-Master" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>Template Name: Subaward Reporting</t>
   </si>
@@ -280,30 +280,38 @@
  "Other"</t>
   </si>
   <si>
-    <t>The Subrecipient's or Contractor's Unique Entity Identifier (UEI) from their SAM.gov profile. 
+    <t>Conditional</t>
+  </si>
+  <si>
+    <t>Explaination if Primary Sector response is "Other"
+Max characters 100</t>
+  </si>
+  <si>
+    <t>Version: 2023.02.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Subrecipient's, Contractor's, or Beneficiary's  Internal Revenue Service (IRS) Taxpayer Identification Number. 
+Format XXXXXXXXX, 
+9 numeric characters.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Subrecipient's or Contractor's Unique Entity Identifier (UEI) from their SAM.gov profile. 
 Format XXXXXXXXXXXX, 
 12 alpha-numeric characters.
-NOTE: One of the following identification numbers must be provided:
--UEI, or
--TIN</t>
-  </si>
-  <si>
-    <t>The Subrecipient's, Contractor's, or Beneficiary's  Internal Revenue Service (IRS) Taxpayer Identification Number. 
-Format XXXXXXXXX, 
-9 numeric characters.
-NOTE: One of the following identification numbers must be provided:
--UEI, or
--TIN</t>
-  </si>
-  <si>
-    <t>Conditional</t>
-  </si>
-  <si>
-    <t>Explaination if Primary Sector response is "Other"
-Max characters 100</t>
-  </si>
-  <si>
-    <t>Version: 2022.12.13</t>
+</t>
+  </si>
+  <si>
+    <t>SubAward/Direct Payment Entity Type</t>
+  </si>
+  <si>
+    <t>The type of entity for this subaward or direct payment. Select one of the predefined menu items:
+"Subrecipient"
+"Contractor"
+"Beneficiary"</t>
+  </si>
+  <si>
+    <t>Entity_Type_2__c</t>
   </si>
 </sst>
 </file>
@@ -348,7 +356,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -412,24 +420,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -458,11 +453,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -680,39 +676,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U979"/>
+  <dimension ref="A1:V979"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.125" customWidth="1"/>
     <col min="2" max="3" width="18.625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.875" customWidth="1"/>
-    <col min="5" max="5" width="186" customWidth="1"/>
-    <col min="6" max="6" width="32.875" customWidth="1"/>
-    <col min="7" max="7" width="25.625" customWidth="1"/>
-    <col min="8" max="8" width="24.25" style="2" customWidth="1"/>
-    <col min="9" max="9" width="76" customWidth="1"/>
-    <col min="10" max="10" width="30.125" customWidth="1"/>
-    <col min="11" max="11" width="67.875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="24.125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="72.625" customWidth="1"/>
-    <col min="14" max="14" width="74.875" customWidth="1"/>
-    <col min="15" max="15" width="28.5" customWidth="1"/>
-    <col min="16" max="16" width="23.625" customWidth="1"/>
-    <col min="17" max="17" width="27.5" customWidth="1"/>
-    <col min="18" max="18" width="22.875" customWidth="1"/>
-    <col min="19" max="19" width="24.625" customWidth="1"/>
-    <col min="20" max="20" width="27.5" customWidth="1"/>
-    <col min="21" max="21" width="44.75" customWidth="1"/>
+    <col min="4" max="4" width="44.5" customWidth="1"/>
+    <col min="5" max="6" width="39.75" customWidth="1"/>
+    <col min="7" max="7" width="32.875" customWidth="1"/>
+    <col min="8" max="8" width="25.625" customWidth="1"/>
+    <col min="9" max="9" width="24.25" style="2" customWidth="1"/>
+    <col min="10" max="10" width="76" customWidth="1"/>
+    <col min="11" max="11" width="30.125" customWidth="1"/>
+    <col min="12" max="12" width="67.875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="24.125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="72.625" customWidth="1"/>
+    <col min="15" max="15" width="74.875" customWidth="1"/>
+    <col min="16" max="16" width="28.5" customWidth="1"/>
+    <col min="17" max="17" width="23.625" customWidth="1"/>
+    <col min="18" max="18" width="27.5" customWidth="1"/>
+    <col min="19" max="19" width="22.875" customWidth="1"/>
+    <col min="20" max="20" width="24.625" customWidth="1"/>
+    <col min="21" max="21" width="27.5" customWidth="1"/>
+    <col min="22" max="22" width="44.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -720,12 +716,12 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="7"/>
+      <c r="K1" s="6"/>
       <c r="L1" s="7"/>
-      <c r="M1" s="6"/>
+      <c r="M1" s="7"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -733,8 +729,9 @@
       <c r="R1" s="6"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -744,12 +741,12 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
+      <c r="K2" s="6"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="6"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
@@ -757,8 +754,9 @@
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>62</v>
       </c>
@@ -768,12 +766,12 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="7"/>
+      <c r="K3" s="6"/>
       <c r="L3" s="7"/>
-      <c r="M3" s="6"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
@@ -781,8 +779,9 @@
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -798,61 +797,64 @@
       <c r="E4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="R4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="S4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="T4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="U4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="V4" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>38</v>
@@ -863,38 +865,38 @@
       <c r="E5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="18" t="s">
         <v>37</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>67</v>
+      <c r="I5" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>37</v>
+        <v>65</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="M5" s="11" t="s">
         <v>37</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>38</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="9" t="s">
         <v>37</v>
@@ -903,20 +905,23 @@
         <v>37</v>
       </c>
       <c r="S5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="T5" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="U5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="V5" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="31.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="31.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -928,64 +933,67 @@
       <c r="E6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="M6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="N6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="R6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="U6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="V6" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="1" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" s="1" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>66</v>
+      <c r="B7" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>40</v>
@@ -993,56 +1001,59 @@
       <c r="E7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="J7" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="K7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="N7" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="O7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="P7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="Q7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="R7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="S7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="S7" s="12" t="s">
+      <c r="T7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="T7" s="12" t="s">
+      <c r="U7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="U7" s="12" t="s">
+      <c r="V7" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1050,12 +1061,12 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="6"/>
+      <c r="M8" s="7"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
@@ -1063,21 +1074,22 @@
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="6"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -1085,14 +1097,15 @@
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Prod release March 20th (#1010)
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/subawardBulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/subawardBulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\Downloads\SLFRFBulkUploadTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\do.treas.gov\dfsres\isilon\Homeshare3\CarrikerCh\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93700437-54C7-442F-B804-12B87FE85BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDE387B-F620-43D9-9B60-E28F315974D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="855" windowWidth="20655" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Award-Reporting-Master" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>Template Name: Subaward Reporting</t>
   </si>
@@ -280,30 +280,38 @@
  "Other"</t>
   </si>
   <si>
-    <t>The Subrecipient's or Contractor's Unique Entity Identifier (UEI) from their SAM.gov profile. 
+    <t>Conditional</t>
+  </si>
+  <si>
+    <t>Explaination if Primary Sector response is "Other"
+Max characters 100</t>
+  </si>
+  <si>
+    <t>Version: 2023.02.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Subrecipient's, Contractor's, or Beneficiary's  Internal Revenue Service (IRS) Taxpayer Identification Number. 
+Format XXXXXXXXX, 
+9 numeric characters.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Subrecipient's or Contractor's Unique Entity Identifier (UEI) from their SAM.gov profile. 
 Format XXXXXXXXXXXX, 
 12 alpha-numeric characters.
-NOTE: One of the following identification numbers must be provided:
--UEI, or
--TIN</t>
-  </si>
-  <si>
-    <t>The Subrecipient's, Contractor's, or Beneficiary's  Internal Revenue Service (IRS) Taxpayer Identification Number. 
-Format XXXXXXXXX, 
-9 numeric characters.
-NOTE: One of the following identification numbers must be provided:
--UEI, or
--TIN</t>
-  </si>
-  <si>
-    <t>Conditional</t>
-  </si>
-  <si>
-    <t>Explaination if Primary Sector response is "Other"
-Max characters 100</t>
-  </si>
-  <si>
-    <t>Version: 2022.12.13</t>
+</t>
+  </si>
+  <si>
+    <t>SubAward/Direct Payment Entity Type</t>
+  </si>
+  <si>
+    <t>The type of entity for this subaward or direct payment. Select one of the predefined menu items:
+"Subrecipient"
+"Contractor"
+"Beneficiary"</t>
+  </si>
+  <si>
+    <t>Entity_Type_2__c</t>
   </si>
 </sst>
 </file>
@@ -348,7 +356,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -412,24 +420,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -458,11 +453,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -680,39 +676,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U979"/>
+  <dimension ref="A1:V979"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.125" customWidth="1"/>
     <col min="2" max="3" width="18.625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="70.875" customWidth="1"/>
-    <col min="5" max="5" width="186" customWidth="1"/>
-    <col min="6" max="6" width="32.875" customWidth="1"/>
-    <col min="7" max="7" width="25.625" customWidth="1"/>
-    <col min="8" max="8" width="24.25" style="2" customWidth="1"/>
-    <col min="9" max="9" width="76" customWidth="1"/>
-    <col min="10" max="10" width="30.125" customWidth="1"/>
-    <col min="11" max="11" width="67.875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="24.125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="72.625" customWidth="1"/>
-    <col min="14" max="14" width="74.875" customWidth="1"/>
-    <col min="15" max="15" width="28.5" customWidth="1"/>
-    <col min="16" max="16" width="23.625" customWidth="1"/>
-    <col min="17" max="17" width="27.5" customWidth="1"/>
-    <col min="18" max="18" width="22.875" customWidth="1"/>
-    <col min="19" max="19" width="24.625" customWidth="1"/>
-    <col min="20" max="20" width="27.5" customWidth="1"/>
-    <col min="21" max="21" width="44.75" customWidth="1"/>
+    <col min="4" max="4" width="44.5" customWidth="1"/>
+    <col min="5" max="6" width="39.75" customWidth="1"/>
+    <col min="7" max="7" width="32.875" customWidth="1"/>
+    <col min="8" max="8" width="25.625" customWidth="1"/>
+    <col min="9" max="9" width="24.25" style="2" customWidth="1"/>
+    <col min="10" max="10" width="76" customWidth="1"/>
+    <col min="11" max="11" width="30.125" customWidth="1"/>
+    <col min="12" max="12" width="67.875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="24.125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="72.625" customWidth="1"/>
+    <col min="15" max="15" width="74.875" customWidth="1"/>
+    <col min="16" max="16" width="28.5" customWidth="1"/>
+    <col min="17" max="17" width="23.625" customWidth="1"/>
+    <col min="18" max="18" width="27.5" customWidth="1"/>
+    <col min="19" max="19" width="22.875" customWidth="1"/>
+    <col min="20" max="20" width="24.625" customWidth="1"/>
+    <col min="21" max="21" width="27.5" customWidth="1"/>
+    <col min="22" max="22" width="44.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -720,12 +716,12 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="7"/>
+      <c r="K1" s="6"/>
       <c r="L1" s="7"/>
-      <c r="M1" s="6"/>
+      <c r="M1" s="7"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -733,8 +729,9 @@
       <c r="R1" s="6"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -744,12 +741,12 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
+      <c r="K2" s="6"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="6"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
@@ -757,8 +754,9 @@
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>62</v>
       </c>
@@ -768,12 +766,12 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="7"/>
+      <c r="K3" s="6"/>
       <c r="L3" s="7"/>
-      <c r="M3" s="6"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
@@ -781,8 +779,9 @@
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -798,61 +797,64 @@
       <c r="E4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="R4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="S4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="T4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="U4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="V4" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>38</v>
@@ -863,38 +865,38 @@
       <c r="E5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="18" t="s">
         <v>37</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>67</v>
+      <c r="I5" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>37</v>
+        <v>65</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="M5" s="11" t="s">
         <v>37</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O5" s="9" t="s">
         <v>38</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="9" t="s">
         <v>37</v>
@@ -903,20 +905,23 @@
         <v>37</v>
       </c>
       <c r="S5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="T5" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="U5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="V5" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="31.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="31.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -928,64 +933,67 @@
       <c r="E6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="M6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="N6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="P6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="R6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="9" t="s">
+      <c r="U6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="V6" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="1" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" s="1" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>66</v>
+      <c r="B7" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>40</v>
@@ -993,56 +1001,59 @@
       <c r="E7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="J7" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="K7" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="N7" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="O7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="P7" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="Q7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="R7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="S7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="S7" s="12" t="s">
+      <c r="T7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="T7" s="12" t="s">
+      <c r="U7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="U7" s="12" t="s">
+      <c r="V7" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1050,12 +1061,12 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="6"/>
+      <c r="M8" s="7"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
@@ -1063,21 +1074,22 @@
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
+      <c r="K9" s="6"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="6"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -1085,14 +1097,15 @@
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
chore: update export templates (v2024-08) (#3433)
* parseOutputTemplates: capture & diff helpText

* yarn parse-output-templates

* yarn parse-output-templates

* yarn parse-output-templates

---------

Co-authored-by: Andrew Hyndman <ajhyndman@outlook.com.au>
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/subawardBulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/subawardBulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd93f4fa04466af4/Desktop/SLFRFBulkUploadTemplates/SLFRFBulkUploadTemplates/SLFRFBulkUploadTemplates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="13_ncr:1_{E9A4FF24-0196-4AB1-9314-4ADA91CCBB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0D430BA-DE7C-472D-B460-7E2DE77760D7}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="13_ncr:1_{E9A4FF24-0196-4AB1-9314-4ADA91CCBB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{325B4C21-4823-4A1E-9773-DD8C7821F498}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub-Award-Reporting-Master" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
   <si>
     <t>Template Name: Subaward Reporting</t>
   </si>
@@ -361,9 +361,6 @@
     <t>Personnel_Estimated_Expended</t>
   </si>
   <si>
-    <t>Personnel_Actual_Expended</t>
-  </si>
-  <si>
     <t>Personnel_Expended_FTE_Count</t>
   </si>
   <si>
@@ -371,9 +368,6 @@
   </si>
   <si>
     <t>Estimated Personnel Expenditures</t>
-  </si>
-  <si>
-    <t>Actual Personnel Expenditures</t>
   </si>
   <si>
     <t>Personnel Expended FTE Count</t>
@@ -384,10 +378,6 @@
 </t>
   </si>
   <si>
-    <t>Actual personnel expenditures in 2025 and 2026 field.
-Required If Subaward Type is Direct Payment and and an amount is entered into the 2025/2026 estimated personnel cost.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of full-time equivalent (FTE) positions for which funds are obligated. 
 Required If Subaward Type is Direct Payment and and an amount is entered into the 2025/2026 estimated personnel cost.
 </t>
@@ -401,16 +391,10 @@
     <t>Contract_Estimated_Expended</t>
   </si>
   <si>
-    <t>Contract_Actual_Expended</t>
-  </si>
-  <si>
     <t>Contract_Expended_Justification</t>
   </si>
   <si>
     <t>Contract Estimated Expended</t>
-  </si>
-  <si>
-    <t>Contract Actual Expended</t>
   </si>
   <si>
     <t>Contract Expended Justfiication</t>
@@ -423,16 +407,6 @@
 “Contract: Blanket Purchase Agreement”
 “Contract: Definitive Contract”
 </t>
-  </si>
-  <si>
-    <t>Actual funds expended to cover change orders and contingencies field.
-Required If Subaward Type is one of the following: 
-“Contract: Purchase Order”
-“Contract: Delivery Order”
-“Contract: Blanket Purchase Agreement”
-“Contract: Definitive Contract”
-AND
- an amount greater than 0 was added to the estimated Admin &amp; Legal expenses.</t>
   </si>
   <si>
     <t>The type of entity for this subaward or direct payment. Select one of the predefined menu items:
@@ -653,10 +627,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -857,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH979"/>
+  <dimension ref="A1:AF979"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -891,15 +861,12 @@
     <col min="26" max="26" width="29.59765625" style="3" customWidth="1"/>
     <col min="27" max="27" width="35.3984375" style="3" customWidth="1"/>
     <col min="28" max="28" width="32.296875" style="3" customWidth="1"/>
-    <col min="29" max="29" width="23.59765625" style="3" customWidth="1"/>
-    <col min="30" max="30" width="28.5" style="3" customWidth="1"/>
-    <col min="31" max="31" width="27.69921875" style="3" customWidth="1"/>
-    <col min="32" max="32" width="29.69921875" style="3" customWidth="1"/>
-    <col min="33" max="33" width="23.59765625" style="3" customWidth="1"/>
-    <col min="34" max="34" width="29.69921875" style="3" customWidth="1"/>
+    <col min="29" max="29" width="28.5" style="3" customWidth="1"/>
+    <col min="30" max="30" width="27.69921875" style="3" customWidth="1"/>
+    <col min="31" max="32" width="29.69921875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>66</v>
       </c>
@@ -932,10 +899,8 @@
       <c r="AD1" s="5"/>
       <c r="AE1" s="5"/>
       <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
     </row>
-    <row r="2" spans="1:34" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -968,10 +933,8 @@
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
       <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
     </row>
-    <row r="3" spans="1:34" ht="141.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" ht="141.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>60</v>
       </c>
@@ -1004,10 +967,8 @@
       <c r="AD3" s="5"/>
       <c r="AE3" s="5"/>
       <c r="AF3" s="5"/>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="5"/>
     </row>
-    <row r="4" spans="1:34" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -1099,19 +1060,13 @@
         <v>86</v>
       </c>
       <c r="AE4" s="10" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="AF4" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="AG4" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="AH4" s="10" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>36</v>
       </c>
@@ -1208,14 +1163,8 @@
       <c r="AF5" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AG5" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH5" s="10" t="s">
-        <v>64</v>
-      </c>
     </row>
-    <row r="6" spans="1:34" ht="31.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" ht="31.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>61</v>
       </c>
@@ -1298,28 +1247,22 @@
         <v>83</v>
       </c>
       <c r="AB6" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC6" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="AC6" s="17" t="s">
-        <v>89</v>
-      </c>
       <c r="AD6" s="17" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="AE6" s="17" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="AF6" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="AG6" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="AH6" s="17" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:34" s="1" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" s="1" customFormat="1" ht="402" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>39</v>
       </c>
@@ -1336,7 +1279,7 @@
         <v>41</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>75</v>
@@ -1372,7 +1315,7 @@
         <v>49</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="S7" s="12" t="s">
         <v>50</v>
@@ -1387,7 +1330,7 @@
         <v>52</v>
       </c>
       <c r="W7" s="12" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="X7" s="19" t="s">
         <v>74</v>
@@ -1399,31 +1342,25 @@
         <v>80</v>
       </c>
       <c r="AA7" s="19" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AB7" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC7" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD7" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="AC7" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD7" s="19" t="s">
-        <v>93</v>
-      </c>
       <c r="AE7" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AF7" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="AG7" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH7" s="19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1454,10 +1391,8 @@
       <c r="AD8" s="5"/>
       <c r="AE8" s="5"/>
       <c r="AF8" s="5"/>
-      <c r="AG8" s="5"/>
-      <c r="AH8" s="5"/>
     </row>
-    <row r="9" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -1488,16 +1423,14 @@
       <c r="AD9" s="13"/>
       <c r="AE9" s="13"/>
       <c r="AF9" s="13"/>
-      <c r="AG9" s="13"/>
-      <c r="AH9" s="13"/>
     </row>
-    <row r="10" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>